<commit_message>
Added work order teams
</commit_message>
<xml_diff>
--- a/lib/i18n/i18n.xlsx
+++ b/lib/i18n/i18n.xlsx
@@ -116,6 +116,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,6 +138,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,7 +214,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Added create safety method and work plan template
</commit_message>
<xml_diff>
--- a/lib/i18n/i18n.xlsx
+++ b/lib/i18n/i18n.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Folder</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>My Work</t>
+  </si>
+  <si>
+    <t>work-template</t>
+  </si>
+  <si>
+    <t>Work Template</t>
+  </si>
+  <si>
+    <t>safety-template</t>
+  </si>
+  <si>
+    <t>Safety Template</t>
   </si>
 </sst>
 </file>
@@ -209,12 +221,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -361,6 +373,28 @@
         <v>28</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>